<commit_message>
Clean up supporting files
</commit_message>
<xml_diff>
--- a/InputData/acronym-key.xlsx
+++ b/InputData/acronym-key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5909EE-E88B-43D7-B664-596C63D1AFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E80D7E-7524-4450-B0EA-386A2396A50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6435" yWindow="1185" windowWidth="21600" windowHeight="22305" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="667">
   <si>
     <t>Top Level Folder</t>
   </si>
@@ -2021,6 +2021,18 @@
   </si>
   <si>
     <t>Annual Vehicle Licensing Registration and Property Tax Costs</t>
+  </si>
+  <si>
+    <t>IHDbT</t>
+  </si>
+  <si>
+    <t>Industrial Heat Demand by Temperature</t>
+  </si>
+  <si>
+    <t>DRCF</t>
+  </si>
+  <si>
+    <t>Demand Response Capacity Factor</t>
   </si>
 </sst>
 </file>
@@ -2587,7 +2599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2919,11 +2931,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H234"/>
+  <dimension ref="A1:H236"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4130,53 +4142,52 @@
         <v>112</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>342</v>
+        <v>665</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>344</v>
-      </c>
+        <v>666</v>
+      </c>
+      <c r="D75" s="3"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F75" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="F76" s="16" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E76" s="3"/>
+      <c r="F76" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>190</v>
+        <v>649</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>112</v>
+        <v>650</v>
+      </c>
+      <c r="F77" s="16" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4184,61 +4195,64 @@
         <v>44</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>541</v>
+        <v>190</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>542</v>
+        <v>191</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>461</v>
+        <v>541</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="F79" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>491</v>
+        <v>461</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+      <c r="F80" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>618</v>
+        <v>491</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>619</v>
-      </c>
-      <c r="F81" s="16" t="s">
-        <v>306</v>
+        <v>490</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4246,58 +4260,58 @@
         <v>44</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>620</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>619</v>
+      </c>
+      <c r="F82" s="16" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>617</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>53</v>
+        <v>317</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>351</v>
+        <v>318</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>354</v>
+        <v>53</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>355</v>
+        <v>64</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>351</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>113</v>
+        <v>222</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4305,78 +4319,78 @@
         <v>44</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>464</v>
+        <v>354</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>465</v>
+        <v>355</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>572</v>
+        <v>464</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>201</v>
+        <v>572</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>651</v>
+        <v>201</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>652</v>
+        <v>200</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>341</v>
+        <v>115</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>54</v>
+        <v>651</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F90" s="4" t="s">
-        <v>112</v>
+        <v>652</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -4384,44 +4398,44 @@
         <v>44</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>233</v>
+        <v>54</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>55</v>
+        <v>233</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>213</v>
+        <v>55</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>112</v>
+        <v>66</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -4429,78 +4443,75 @@
         <v>44</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F95" s="6" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>527</v>
+        <v>240</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>528</v>
+        <v>241</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>601</v>
+        <v>527</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>602</v>
+        <v>528</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>529</v>
       </c>
       <c r="F97" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>216</v>
+        <v>601</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F98" s="14" t="s">
-        <v>298</v>
+        <v>602</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4508,13 +4519,16 @@
         <v>44</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F99" s="4" t="s">
-        <v>112</v>
+        <v>217</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F99" s="14" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4522,48 +4536,48 @@
         <v>44</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F100" s="6" t="s">
+      <c r="F101" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="19" t="s">
+    <row r="102" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B101" s="19" t="s">
+      <c r="B102" s="19" t="s">
         <v>409</v>
       </c>
-      <c r="C101" s="19" t="s">
+      <c r="C102" s="19" t="s">
         <v>410</v>
       </c>
-      <c r="D101" s="19" t="s">
+      <c r="D102" s="19" t="s">
         <v>411</v>
       </c>
-      <c r="E101" s="19"/>
-      <c r="F101" s="23" t="s">
+      <c r="E102" s="19"/>
+      <c r="F102" s="23" t="s">
         <v>360</v>
       </c>
-      <c r="G101" s="19" t="s">
+      <c r="G102" s="19" t="s">
         <v>412</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="F102" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -4571,10 +4585,10 @@
         <v>325</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="F103" s="5" t="s">
         <v>113</v>
@@ -4585,10 +4599,10 @@
         <v>325</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F104" s="5" t="s">
         <v>113</v>
@@ -4599,10 +4613,10 @@
         <v>325</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F105" s="5" t="s">
         <v>113</v>
@@ -4613,151 +4627,151 @@
         <v>325</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>325</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>493</v>
+        <v>327</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="F107" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>325</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>208</v>
+        <v>493</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F108" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>325</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F109" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="19" t="s">
+    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B110" s="19" t="s">
+      <c r="B110" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="B111" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="C110" s="19" t="s">
+      <c r="C111" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="D110" s="19"/>
-      <c r="E110" s="19"/>
-      <c r="F110" s="22" t="s">
+      <c r="D111" s="19"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="G110" s="19"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B111" s="27" t="s">
-        <v>553</v>
-      </c>
-      <c r="C111" s="27" t="s">
-        <v>554</v>
-      </c>
-      <c r="D111" s="27"/>
-      <c r="E111" s="27"/>
-      <c r="F111" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G111" s="27"/>
+      <c r="G111" s="19"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>557</v>
-      </c>
+      <c r="B112" s="27" t="s">
+        <v>553</v>
+      </c>
+      <c r="C112" s="27" t="s">
+        <v>554</v>
+      </c>
+      <c r="D112" s="27"/>
+      <c r="E112" s="27"/>
       <c r="F112" s="4" t="s">
         <v>112</v>
       </c>
+      <c r="G112" s="27"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>442</v>
+        <v>555</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>443</v>
+        <v>556</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>557</v>
       </c>
       <c r="F113" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>69</v>
+        <v>442</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>316</v>
+        <v>443</v>
       </c>
       <c r="F114" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>370</v>
+        <v>69</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F115" s="6" t="s">
-        <v>114</v>
+        <v>72</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4765,13 +4779,13 @@
         <v>68</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>641</v>
+        <v>370</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>642</v>
-      </c>
-      <c r="F116" s="4" t="s">
-        <v>112</v>
+        <v>371</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -4779,64 +4793,61 @@
         <v>68</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>621</v>
+        <v>641</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="F117" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>642</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>70</v>
+        <v>621</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F118" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="G118" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>368</v>
+        <v>70</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="F119" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="F119" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>452</v>
+        <v>368</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="F120" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="G120" s="2" t="s">
-        <v>458</v>
+        <v>369</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4844,16 +4855,16 @@
         <v>68</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F121" s="18" t="s">
         <v>360</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4861,133 +4872,136 @@
         <v>68</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F122" s="18" t="s">
         <v>360</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B123" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="F123" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="D124" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F123" s="4" t="s">
+      <c r="F124" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A124" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B124" s="27" t="s">
-        <v>438</v>
-      </c>
-      <c r="C124" s="27" t="s">
-        <v>398</v>
-      </c>
-      <c r="D124" s="27" t="s">
-        <v>399</v>
-      </c>
-      <c r="E124" s="27"/>
-      <c r="F124" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="G124" s="27"/>
-    </row>
-    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" s="27" t="s">
         <v>68</v>
       </c>
       <c r="B125" s="27" t="s">
+        <v>438</v>
+      </c>
+      <c r="C125" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="D125" s="27" t="s">
+        <v>399</v>
+      </c>
+      <c r="E125" s="27"/>
+      <c r="F125" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G125" s="27"/>
+    </row>
+    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B126" s="27" t="s">
         <v>450</v>
       </c>
-      <c r="C125" s="27" t="s">
+      <c r="C126" s="27" t="s">
         <v>451</v>
       </c>
-      <c r="D125" s="27"/>
-      <c r="E125" s="27"/>
-      <c r="F125" s="37" t="s">
+      <c r="D126" s="27"/>
+      <c r="E126" s="27"/>
+      <c r="F126" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="G125" s="27"/>
-    </row>
-    <row r="126" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="2" t="s">
+      <c r="G126" s="27"/>
+    </row>
+    <row r="127" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B127" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C127" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="F126" s="25" t="s">
+      <c r="F127" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="G126" s="2" t="s">
+      <c r="G127" s="2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="33" t="s">
+    <row r="128" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="33" t="s">
         <v>471</v>
       </c>
-      <c r="B127" s="33" t="s">
+      <c r="B128" s="33" t="s">
         <v>473</v>
       </c>
-      <c r="C127" s="33" t="s">
+      <c r="C128" s="33" t="s">
         <v>474</v>
       </c>
-      <c r="D127" s="33" t="s">
+      <c r="D128" s="33" t="s">
         <v>475</v>
       </c>
-      <c r="E127" s="33"/>
-      <c r="F127" s="21" t="s">
+      <c r="E128" s="33"/>
+      <c r="F128" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="G127" s="33"/>
-    </row>
-    <row r="128" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="13" t="s">
-        <v>419</v>
-      </c>
-      <c r="B128" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="C128" s="13" t="s">
-        <v>428</v>
-      </c>
-      <c r="F128" s="6" t="s">
-        <v>114</v>
-      </c>
+      <c r="G128" s="33"/>
     </row>
     <row r="129" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
         <v>419</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C129" s="13" t="s">
-        <v>429</v>
-      </c>
-      <c r="F129" s="5" t="s">
-        <v>113</v>
+        <v>428</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="130" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4995,27 +5009,24 @@
         <v>419</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F130" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="131" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
         <v>419</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C131" s="13" t="s">
-        <v>431</v>
-      </c>
-      <c r="D131" s="13" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F131" s="5" t="s">
         <v>113</v>
@@ -5026,133 +5037,136 @@
         <v>419</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>432</v>
+        <v>431</v>
+      </c>
+      <c r="D132" s="13" t="s">
+        <v>435</v>
       </c>
       <c r="F132" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="133" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
         <v>419</v>
       </c>
       <c r="B133" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="C133" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="B134" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="C133" s="13" t="s">
+      <c r="C134" s="13" t="s">
         <v>433</v>
       </c>
-      <c r="F133" s="7" t="s">
+      <c r="F134" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="G133" s="13" t="s">
+      <c r="G134" s="13" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="134" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A134" s="29" t="s">
+    <row r="135" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="29" t="s">
         <v>419</v>
       </c>
-      <c r="B134" s="29" t="s">
+      <c r="B135" s="29" t="s">
         <v>427</v>
       </c>
-      <c r="C134" s="29" t="s">
+      <c r="C135" s="29" t="s">
         <v>434</v>
       </c>
-      <c r="D134" s="29"/>
-      <c r="E134" s="29"/>
-      <c r="F134" s="36" t="s">
+      <c r="D135" s="29"/>
+      <c r="E135" s="29"/>
+      <c r="F135" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="G134" s="29" t="s">
+      <c r="G135" s="29" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="135" spans="1:7" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="24" t="s">
+    <row r="136" spans="1:7" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="24" t="s">
         <v>419</v>
       </c>
-      <c r="B135" s="24" t="s">
+      <c r="B136" s="24" t="s">
         <v>585</v>
       </c>
-      <c r="C135" s="24" t="s">
+      <c r="C136" s="24" t="s">
         <v>586</v>
       </c>
-      <c r="D135" s="24"/>
-      <c r="E135" s="24"/>
-      <c r="F135" s="22" t="s">
+      <c r="D136" s="24"/>
+      <c r="E136" s="24"/>
+      <c r="F136" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="G135" s="24"/>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
+      <c r="G136" s="24"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B137" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C137" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="F136" s="14" t="s">
+      <c r="F137" s="14" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A137" s="27" t="s">
+    <row r="138" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B137" s="27" t="s">
+      <c r="B138" s="27" t="s">
         <v>610</v>
       </c>
-      <c r="C137" s="27" t="s">
+      <c r="C138" s="27" t="s">
         <v>611</v>
       </c>
-      <c r="D137" s="27" t="s">
+      <c r="D138" s="27" t="s">
         <v>612</v>
       </c>
-      <c r="E137" s="27"/>
-      <c r="F137" s="30" t="s">
+      <c r="E138" s="27"/>
+      <c r="F138" s="30" t="s">
         <v>467</v>
       </c>
-      <c r="G137" s="27"/>
-    </row>
-    <row r="138" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E138" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F138" s="31" t="s">
-        <v>360</v>
-      </c>
-      <c r="G138" s="2" t="s">
-        <v>397</v>
-      </c>
+      <c r="G138" s="27"/>
     </row>
     <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>384</v>
+        <v>234</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="F139" s="6" t="s">
-        <v>114</v>
+        <v>235</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F139" s="31" t="s">
+        <v>360</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5160,10 +5174,10 @@
         <v>76</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>589</v>
+        <v>384</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>590</v>
+        <v>385</v>
       </c>
       <c r="F140" s="6" t="s">
         <v>114</v>
@@ -5174,27 +5188,27 @@
         <v>76</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>77</v>
+        <v>589</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F141" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+        <v>590</v>
+      </c>
+      <c r="F141" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>583</v>
+        <v>77</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="F142" s="6" t="s">
-        <v>114</v>
+        <v>80</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -5202,75 +5216,72 @@
         <v>76</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>78</v>
+        <v>583</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F143" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="G143" s="2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>584</v>
+      </c>
+      <c r="F143" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>607</v>
+        <v>78</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="F144" s="7" t="s">
-        <v>115</v>
+        <v>81</v>
+      </c>
+      <c r="F144" s="18" t="s">
+        <v>360</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>236</v>
+        <v>607</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F145" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>608</v>
+      </c>
+      <c r="F145" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>79</v>
+        <v>663</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="F146" s="30" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>664</v>
+      </c>
+      <c r="F146" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="F147" s="5" t="s">
         <v>113</v>
@@ -5281,13 +5292,16 @@
         <v>76</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>331</v>
+        <v>79</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="F148" s="6" t="s">
-        <v>114</v>
+        <v>82</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F148" s="30" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5295,13 +5309,13 @@
         <v>76</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>332</v>
+        <v>227</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="F149" s="6" t="s">
-        <v>114</v>
+        <v>228</v>
+      </c>
+      <c r="F149" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5309,143 +5323,137 @@
         <v>76</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F150" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F151" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C150" s="2" t="s">
+      <c r="C152" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="F150" s="5" t="s">
+      <c r="F152" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A151" s="27" t="s">
+    <row r="153" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B151" s="27" t="s">
+      <c r="B153" s="27" t="s">
         <v>560</v>
       </c>
-      <c r="C151" s="27" t="s">
+      <c r="C153" s="27" t="s">
         <v>559</v>
       </c>
-      <c r="D151" s="27"/>
-      <c r="E151" s="27"/>
-      <c r="F151" s="28" t="s">
+      <c r="D153" s="27"/>
+      <c r="E153" s="27"/>
+      <c r="F153" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="G151" s="27"/>
-    </row>
-    <row r="152" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A152" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B152" s="27" t="s">
-        <v>579</v>
-      </c>
-      <c r="C152" s="27" t="s">
-        <v>580</v>
-      </c>
-      <c r="D152" s="27"/>
-      <c r="E152" s="27"/>
-      <c r="F152" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="G152" s="27"/>
-    </row>
-    <row r="153" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B153" s="19" t="s">
-        <v>581</v>
-      </c>
-      <c r="C153" s="19" t="s">
-        <v>582</v>
-      </c>
-      <c r="D153" s="19"/>
-      <c r="E153" s="19"/>
-      <c r="F153" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="G153" s="19"/>
+      <c r="G153" s="27"/>
     </row>
     <row r="154" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="27" t="s">
-        <v>495</v>
-      </c>
-      <c r="B154" s="32" t="s">
-        <v>637</v>
-      </c>
-      <c r="C154" s="32" t="s">
-        <v>638</v>
-      </c>
-      <c r="D154" s="32"/>
-      <c r="E154" s="32"/>
-      <c r="F154" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G154" s="32"/>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" s="27" t="s">
-        <v>495</v>
-      </c>
-      <c r="B155" s="27" t="s">
-        <v>503</v>
-      </c>
-      <c r="C155" s="27" t="s">
-        <v>504</v>
-      </c>
-      <c r="D155" s="27"/>
-      <c r="E155" s="27"/>
-      <c r="F155" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G155" s="27"/>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="B154" s="27" t="s">
+        <v>579</v>
+      </c>
+      <c r="C154" s="27" t="s">
+        <v>580</v>
+      </c>
+      <c r="D154" s="27"/>
+      <c r="E154" s="27"/>
+      <c r="F154" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G154" s="27"/>
+    </row>
+    <row r="155" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B155" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="C155" s="19" t="s">
+        <v>582</v>
+      </c>
+      <c r="D155" s="19"/>
+      <c r="E155" s="19"/>
+      <c r="F155" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G155" s="19"/>
+    </row>
+    <row r="156" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="27" t="s">
         <v>495</v>
       </c>
-      <c r="B156" s="27" t="s">
-        <v>505</v>
-      </c>
-      <c r="C156" s="27" t="s">
-        <v>506</v>
-      </c>
-      <c r="D156" s="27"/>
-      <c r="E156" s="27"/>
-      <c r="F156" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G156" s="27"/>
+      <c r="B156" s="32" t="s">
+        <v>637</v>
+      </c>
+      <c r="C156" s="32" t="s">
+        <v>638</v>
+      </c>
+      <c r="D156" s="32"/>
+      <c r="E156" s="32"/>
+      <c r="F156" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G156" s="32"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="27" t="s">
         <v>495</v>
       </c>
-      <c r="B157" s="32" t="s">
-        <v>468</v>
-      </c>
-      <c r="C157" s="32" t="s">
-        <v>469</v>
-      </c>
-      <c r="D157" s="32"/>
-      <c r="E157" s="32"/>
+      <c r="B157" s="27" t="s">
+        <v>503</v>
+      </c>
+      <c r="C157" s="27" t="s">
+        <v>504</v>
+      </c>
+      <c r="D157" s="27"/>
+      <c r="E157" s="27"/>
       <c r="F157" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G157" s="32"/>
+      <c r="G157" s="27"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="27" t="s">
         <v>495</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C158" s="27" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D158" s="27"/>
       <c r="E158" s="27"/>
@@ -5458,99 +5466,97 @@
       <c r="A159" s="27" t="s">
         <v>495</v>
       </c>
-      <c r="B159" s="27" t="s">
-        <v>645</v>
-      </c>
-      <c r="C159" s="27" t="s">
-        <v>646</v>
-      </c>
-      <c r="D159" s="27"/>
-      <c r="E159" s="27" t="s">
-        <v>509</v>
-      </c>
+      <c r="B159" s="32" t="s">
+        <v>468</v>
+      </c>
+      <c r="C159" s="32" t="s">
+        <v>469</v>
+      </c>
+      <c r="D159" s="32"/>
+      <c r="E159" s="32"/>
       <c r="F159" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G159" s="27"/>
-    </row>
-    <row r="160" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G159" s="32"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="27" t="s">
         <v>495</v>
       </c>
       <c r="B160" s="27" t="s">
-        <v>538</v>
+        <v>507</v>
       </c>
       <c r="C160" s="27" t="s">
-        <v>539</v>
-      </c>
-      <c r="D160" s="27" t="s">
-        <v>540</v>
-      </c>
+        <v>508</v>
+      </c>
+      <c r="D160" s="27"/>
       <c r="E160" s="27"/>
       <c r="F160" s="4" t="s">
         <v>112</v>
       </c>
       <c r="G160" s="27"/>
     </row>
-    <row r="161" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="27" t="s">
         <v>495</v>
       </c>
       <c r="B161" s="27" t="s">
+        <v>645</v>
+      </c>
+      <c r="C161" s="27" t="s">
+        <v>646</v>
+      </c>
+      <c r="D161" s="27"/>
+      <c r="E161" s="27" t="s">
         <v>509</v>
       </c>
-      <c r="C161" s="27" t="s">
-        <v>510</v>
-      </c>
-      <c r="F161" s="37" t="s">
+      <c r="F161" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G161" s="27"/>
+    </row>
+    <row r="162" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="27" t="s">
         <v>495</v>
       </c>
       <c r="B162" s="27" t="s">
-        <v>497</v>
+        <v>538</v>
       </c>
       <c r="C162" s="27" t="s">
-        <v>499</v>
-      </c>
-      <c r="D162" s="27"/>
+        <v>539</v>
+      </c>
+      <c r="D162" s="27" t="s">
+        <v>540</v>
+      </c>
       <c r="E162" s="27"/>
       <c r="F162" s="4" t="s">
         <v>112</v>
       </c>
       <c r="G162" s="27"/>
     </row>
-    <row r="163" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="27" t="s">
         <v>495</v>
       </c>
       <c r="B163" s="27" t="s">
-        <v>626</v>
+        <v>509</v>
       </c>
       <c r="C163" s="27" t="s">
-        <v>627</v>
-      </c>
-      <c r="D163" s="27"/>
-      <c r="E163" s="27"/>
-      <c r="F163" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="G163" s="27" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+      <c r="F163" s="37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="27" t="s">
         <v>495</v>
       </c>
       <c r="B164" s="27" t="s">
-        <v>577</v>
+        <v>497</v>
       </c>
       <c r="C164" s="27" t="s">
-        <v>578</v>
+        <v>499</v>
       </c>
       <c r="D164" s="27"/>
       <c r="E164" s="27"/>
@@ -5564,54 +5570,52 @@
         <v>495</v>
       </c>
       <c r="B165" s="27" t="s">
-        <v>563</v>
+        <v>626</v>
       </c>
       <c r="C165" s="27" t="s">
-        <v>564</v>
-      </c>
-      <c r="D165" s="27" t="s">
-        <v>565</v>
-      </c>
+        <v>627</v>
+      </c>
+      <c r="D165" s="27"/>
       <c r="E165" s="27"/>
-      <c r="F165" s="4"/>
-      <c r="G165" s="27"/>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F165" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="G165" s="27" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="27" t="s">
         <v>495</v>
       </c>
       <c r="B166" s="27" t="s">
-        <v>624</v>
+        <v>577</v>
       </c>
       <c r="C166" s="27" t="s">
-        <v>625</v>
+        <v>578</v>
       </c>
       <c r="D166" s="27"/>
       <c r="E166" s="27"/>
-      <c r="F166" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="G166" s="27" t="s">
-        <v>629</v>
-      </c>
+      <c r="F166" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G166" s="27"/>
     </row>
     <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="27" t="s">
         <v>495</v>
       </c>
       <c r="B167" s="27" t="s">
-        <v>591</v>
+        <v>563</v>
       </c>
       <c r="C167" s="27" t="s">
-        <v>592</v>
-      </c>
-      <c r="D167" s="27"/>
-      <c r="E167" s="27" t="s">
-        <v>497</v>
-      </c>
-      <c r="F167" s="4" t="s">
-        <v>112</v>
-      </c>
+        <v>564</v>
+      </c>
+      <c r="D167" s="27" t="s">
+        <v>565</v>
+      </c>
+      <c r="E167" s="27"/>
+      <c r="F167" s="4"/>
       <c r="G167" s="27"/>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -5619,32 +5623,36 @@
         <v>495</v>
       </c>
       <c r="B168" s="27" t="s">
-        <v>587</v>
+        <v>624</v>
       </c>
       <c r="C168" s="27" t="s">
-        <v>588</v>
+        <v>625</v>
       </c>
       <c r="D168" s="27"/>
       <c r="E168" s="27"/>
-      <c r="F168" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G168" s="27"/>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F168" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="G168" s="27" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="27" t="s">
         <v>495</v>
       </c>
       <c r="B169" s="27" t="s">
-        <v>498</v>
+        <v>591</v>
       </c>
       <c r="C169" s="27" t="s">
-        <v>500</v>
+        <v>592</v>
       </c>
       <c r="D169" s="27"/>
-      <c r="E169" s="27"/>
-      <c r="F169" s="6" t="s">
-        <v>114</v>
+      <c r="E169" s="27" t="s">
+        <v>497</v>
+      </c>
+      <c r="F169" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="G169" s="27"/>
     </row>
@@ -5653,10 +5661,10 @@
         <v>495</v>
       </c>
       <c r="B170" s="27" t="s">
-        <v>549</v>
+        <v>587</v>
       </c>
       <c r="C170" s="27" t="s">
-        <v>550</v>
+        <v>588</v>
       </c>
       <c r="D170" s="27"/>
       <c r="E170" s="27"/>
@@ -5670,10 +5678,10 @@
         <v>495</v>
       </c>
       <c r="B171" s="27" t="s">
-        <v>551</v>
+        <v>498</v>
       </c>
       <c r="C171" s="27" t="s">
-        <v>552</v>
+        <v>500</v>
       </c>
       <c r="D171" s="27"/>
       <c r="E171" s="27"/>
@@ -5687,114 +5695,117 @@
         <v>495</v>
       </c>
       <c r="B172" s="27" t="s">
-        <v>639</v>
+        <v>549</v>
       </c>
       <c r="C172" s="27" t="s">
-        <v>640</v>
+        <v>550</v>
       </c>
       <c r="D172" s="27"/>
       <c r="E172" s="27"/>
-      <c r="F172" s="4" t="s">
-        <v>112</v>
+      <c r="F172" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="G172" s="27"/>
     </row>
-    <row r="173" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="27" t="s">
         <v>495</v>
       </c>
       <c r="B173" s="27" t="s">
-        <v>501</v>
+        <v>551</v>
       </c>
       <c r="C173" s="27" t="s">
-        <v>502</v>
+        <v>552</v>
       </c>
       <c r="D173" s="27"/>
       <c r="E173" s="27"/>
-      <c r="F173" s="18" t="s">
+      <c r="F173" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G173" s="27"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="27" t="s">
+        <v>495</v>
+      </c>
+      <c r="B174" s="27" t="s">
+        <v>639</v>
+      </c>
+      <c r="C174" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="D174" s="27"/>
+      <c r="E174" s="27"/>
+      <c r="F174" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G174" s="27"/>
+    </row>
+    <row r="175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A175" s="27" t="s">
+        <v>495</v>
+      </c>
+      <c r="B175" s="27" t="s">
+        <v>501</v>
+      </c>
+      <c r="C175" s="27" t="s">
+        <v>502</v>
+      </c>
+      <c r="D175" s="27"/>
+      <c r="E175" s="27"/>
+      <c r="F175" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="G173" s="27" t="s">
+      <c r="G175" s="27" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="19" t="s">
+    <row r="176" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="19" t="s">
         <v>495</v>
       </c>
-      <c r="B174" s="19" t="s">
+      <c r="B176" s="19" t="s">
         <v>575</v>
       </c>
-      <c r="C174" s="19" t="s">
+      <c r="C176" s="19" t="s">
         <v>576</v>
       </c>
-      <c r="D174" s="19"/>
-      <c r="E174" s="19"/>
-      <c r="F174" s="21" t="s">
+      <c r="D176" s="19"/>
+      <c r="E176" s="19"/>
+      <c r="F176" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="G174" s="19"/>
-    </row>
-    <row r="175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F175" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="E176" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F176" s="14" t="s">
-        <v>298</v>
-      </c>
+      <c r="G176" s="19"/>
     </row>
     <row r="177" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F177" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>250</v>
+        <v>361</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="F178" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="G178" s="2" t="s">
-        <v>408</v>
+        <v>362</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F178" s="14" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5802,27 +5813,30 @@
         <v>106</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="F179" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>107</v>
+        <v>250</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F180" s="6" t="s">
-        <v>114</v>
+        <v>251</v>
+      </c>
+      <c r="F180" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="G180" s="2" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5830,156 +5844,156 @@
         <v>106</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="F181" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="F181" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>255</v>
+        <v>107</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="F182" s="14" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F182" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B183" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C183" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D183" s="19"/>
-      <c r="E183" s="19"/>
-      <c r="F183" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="G183" s="19"/>
+      <c r="B183" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F183" s="4" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="184" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="F184" s="14" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B185" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C185" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D185" s="19"/>
+      <c r="E185" s="19"/>
+      <c r="F185" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G185" s="19"/>
+    </row>
+    <row r="186" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B186" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="C186" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F184" s="7" t="s">
+      <c r="F186" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="G184" s="2" t="s">
+      <c r="G186" s="2" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
+    <row r="187" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B187" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C185" s="2" t="s">
+      <c r="C187" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F185" s="7" t="s">
+      <c r="F187" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="G185" s="2" t="s">
+      <c r="G187" s="2" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="19" t="s">
+    <row r="188" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B186" s="19" t="s">
+      <c r="B188" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="C186" s="19" t="s">
+      <c r="C188" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="D186" s="19"/>
-      <c r="E186" s="19"/>
-      <c r="F186" s="25" t="s">
+      <c r="D188" s="19"/>
+      <c r="E188" s="19"/>
+      <c r="F188" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="G186" s="19" t="s">
+      <c r="G188" s="19" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" s="27" t="s">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B187" s="27" t="s">
+      <c r="B189" s="27" t="s">
         <v>657</v>
       </c>
-      <c r="C187" s="27" t="s">
+      <c r="C189" s="27" t="s">
         <v>658</v>
       </c>
-      <c r="D187" s="27"/>
-      <c r="E187" s="27"/>
-      <c r="F187" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G187" s="27"/>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C188" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F188" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A189" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="D189" s="27"/>
+      <c r="E189" s="27"/>
       <c r="F189" s="6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G189" s="27"/>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>661</v>
+        <v>87</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="F190" s="6" t="s">
-        <v>114</v>
+        <v>95</v>
+      </c>
+      <c r="F190" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -5987,24 +6001,24 @@
         <v>86</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>482</v>
+        <v>88</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="F191" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="F191" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="F192" s="6" t="s">
         <v>114</v>
@@ -6015,13 +6029,13 @@
         <v>86</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>337</v>
+        <v>482</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="F193" s="4" t="s">
-        <v>112</v>
+        <v>483</v>
+      </c>
+      <c r="F193" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -6029,24 +6043,24 @@
         <v>86</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>647</v>
+        <v>659</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="F194" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>660</v>
+      </c>
+      <c r="F194" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>304</v>
+        <v>337</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>305</v>
+        <v>338</v>
       </c>
       <c r="F195" s="4" t="s">
         <v>112</v>
@@ -6057,13 +6071,13 @@
         <v>86</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>268</v>
+        <v>647</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="F196" s="4" t="s">
-        <v>112</v>
+        <v>648</v>
+      </c>
+      <c r="F196" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="197" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6071,16 +6085,13 @@
         <v>86</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>282</v>
+        <v>304</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E197" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="F197" s="6" t="s">
-        <v>114</v>
+        <v>305</v>
+      </c>
+      <c r="F197" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
@@ -6088,27 +6099,30 @@
         <v>86</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F198" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="F199" s="4" t="s">
-        <v>112</v>
+        <v>283</v>
+      </c>
+      <c r="E199" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="F199" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
@@ -6116,27 +6130,27 @@
         <v>86</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F200" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="201" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+      <c r="F200" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="F201" s="6" t="s">
-        <v>286</v>
+        <v>271</v>
+      </c>
+      <c r="F201" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
@@ -6144,27 +6158,27 @@
         <v>86</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F202" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>405</v>
+        <v>284</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>406</v>
+        <v>285</v>
       </c>
       <c r="F203" s="6" t="s">
-        <v>114</v>
+        <v>286</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -6172,30 +6186,27 @@
         <v>86</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F204" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A205" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="F204" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B205" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="C205" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="F205" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="G205" s="2" t="s">
-        <v>392</v>
+      <c r="B205" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F205" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -6203,27 +6214,30 @@
         <v>86</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>403</v>
+        <v>289</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>404</v>
+        <v>290</v>
       </c>
       <c r="F206" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A207" s="2" t="s">
+    <row r="207" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A207" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B207" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F207" s="6" t="s">
-        <v>114</v>
+      <c r="B207" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="C207" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="F207" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="G207" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
@@ -6231,13 +6245,13 @@
         <v>86</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>90</v>
+        <v>403</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F208" s="6" t="s">
-        <v>114</v>
+        <v>404</v>
+      </c>
+      <c r="F208" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
@@ -6245,10 +6259,10 @@
         <v>86</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F209" s="6" t="s">
         <v>114</v>
@@ -6259,13 +6273,13 @@
         <v>86</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F210" s="5" t="s">
-        <v>113</v>
+        <v>98</v>
+      </c>
+      <c r="F210" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -6273,13 +6287,13 @@
         <v>86</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>523</v>
+        <v>91</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="F211" s="5" t="s">
-        <v>113</v>
+        <v>99</v>
+      </c>
+      <c r="F211" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -6287,10 +6301,10 @@
         <v>86</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>561</v>
+        <v>92</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>562</v>
+        <v>100</v>
       </c>
       <c r="F212" s="5" t="s">
         <v>113</v>
@@ -6301,13 +6315,13 @@
         <v>86</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>93</v>
+        <v>523</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F213" s="4" t="s">
-        <v>112</v>
+        <v>524</v>
+      </c>
+      <c r="F213" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -6315,47 +6329,41 @@
         <v>86</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>655</v>
+        <v>561</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>656</v>
-      </c>
-      <c r="F214" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="215" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>562</v>
+      </c>
+      <c r="F214" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>347</v>
+        <v>93</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="F215" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="G215" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="216" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="F215" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>349</v>
+        <v>655</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="F216" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="G216" s="2" t="s">
-        <v>393</v>
+        <v>656</v>
+      </c>
+      <c r="F216" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="217" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6363,10 +6371,10 @@
         <v>86</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>287</v>
+        <v>347</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>288</v>
+        <v>348</v>
       </c>
       <c r="F217" s="18" t="s">
         <v>360</v>
@@ -6375,80 +6383,86 @@
         <v>393</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>276</v>
+        <v>349</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E218" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="F218" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="219" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+      <c r="F218" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="G218" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>94</v>
+        <v>287</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F219" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="220" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="F219" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="G219" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>518</v>
+        <v>276</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="F220" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="G220" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+      <c r="E220" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F220" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>595</v>
+        <v>94</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="F221" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="F221" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>293</v>
+        <v>518</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F222" s="16" t="s">
-        <v>306</v>
+        <v>519</v>
+      </c>
+      <c r="F222" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G222" s="2" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
@@ -6456,10 +6470,10 @@
         <v>86</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>353</v>
+        <v>595</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>352</v>
+        <v>596</v>
       </c>
       <c r="F223" s="6" t="s">
         <v>114</v>
@@ -6470,13 +6484,13 @@
         <v>86</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F224" s="6" t="s">
-        <v>114</v>
+        <v>294</v>
+      </c>
+      <c r="F224" s="16" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
@@ -6484,13 +6498,13 @@
         <v>86</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>272</v>
+        <v>353</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F225" s="14" t="s">
-        <v>298</v>
+        <v>352</v>
+      </c>
+      <c r="F225" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -6498,13 +6512,13 @@
         <v>86</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>615</v>
+        <v>280</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="F226" s="16" t="s">
-        <v>306</v>
+        <v>281</v>
+      </c>
+      <c r="F226" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -6512,16 +6526,13 @@
         <v>86</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>613</v>
+        <v>272</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="E227" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="F227" s="6" t="s">
-        <v>114</v>
+        <v>273</v>
+      </c>
+      <c r="F227" s="14" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -6529,78 +6540,75 @@
         <v>86</v>
       </c>
       <c r="B228" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="F228" s="16" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="E229" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F229" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B230" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C228" s="2" t="s">
+      <c r="C230" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="F228" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="229" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B229" s="19" t="s">
-        <v>363</v>
-      </c>
-      <c r="C229" s="19" t="s">
-        <v>364</v>
-      </c>
-      <c r="D229" s="19"/>
-      <c r="E229" s="19"/>
-      <c r="F229" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="G229" s="19"/>
-    </row>
-    <row r="230" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A230" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C230" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D230" s="2" t="s">
-        <v>372</v>
       </c>
       <c r="F230" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A231" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B231" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D231" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="F231" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="232" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A231" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B231" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="C231" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="D231" s="19"/>
+      <c r="E231" s="19"/>
+      <c r="F231" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G231" s="19"/>
+    </row>
+    <row r="232" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>295</v>
+        <v>104</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>296</v>
+        <v>105</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>297</v>
+        <v>372</v>
       </c>
       <c r="F232" s="6" t="s">
         <v>114</v>
@@ -6611,33 +6619,67 @@
         <v>103</v>
       </c>
       <c r="B233" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D233" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F233" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D234" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F234" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B235" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="C233" s="2" t="s">
+      <c r="C235" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="F233" s="5" t="s">
+      <c r="F235" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="19" t="s">
+    <row r="236" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B234" s="19" t="s">
+      <c r="B236" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="C234" s="19" t="s">
+      <c r="C236" s="19" t="s">
         <v>346</v>
       </c>
-      <c r="D234" s="19" t="s">
+      <c r="D236" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="E234" s="19"/>
-      <c r="F234" s="20" t="s">
+      <c r="E236" s="19"/>
+      <c r="F236" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="G234" s="19"/>
+      <c r="G236" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>